<commit_message>
Updated 100-Pin Variant BOM.xlsx
Fixed document sensitivity tag on V100P BOM.xlsx from "protected" to "Public"
</commit_message>
<xml_diff>
--- a/hardware/STM32_100pin_Variant/BOM.xlsx
+++ b/hardware/STM32_100pin_Variant/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toyotawill/Documents/Projects/RAMN/RAMN_STM32_100pin/hardware/STM32_100pin_Variant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydocs.toyota.com/personal/william_greenfield_toyota_com/Documents/Projects/RAMN/RAMN_STM32_100pin/hardware/STM32_100pin_Variant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BEB3EB33-8E9C-DA44-857D-66C9E1957344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{BEB3EB33-8E9C-DA44-857D-66C9E1957344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8600F7D5-99B6-41E3-9518-FD1FD98B6D1B}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27080"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ramn" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -792,12 +792,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1152,25 +1151,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="33.125" customWidth="1"/>
+    <col min="3" max="3" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="5" max="5" width="30.125" customWidth="1"/>
+    <col min="6" max="6" width="32.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1181,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1196,7 +1194,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1209,7 +1207,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1220,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1235,7 +1233,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1258,7 +1256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1277,7 +1275,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1299,7 +1297,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1321,7 +1319,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1342,7 +1340,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1363,7 +1361,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1384,7 +1382,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1405,7 +1403,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1426,7 +1424,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1447,7 +1445,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -1468,7 +1466,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1487,7 +1485,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1508,7 +1506,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -1529,7 +1527,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -1550,7 +1548,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
@@ -1571,7 +1569,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
@@ -1592,7 +1590,7 @@
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
@@ -1611,7 +1609,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>71</v>
       </c>
@@ -1630,7 +1628,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -1649,7 +1647,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -1670,7 +1668,7 @@
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -1691,7 +1689,7 @@
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>83</v>
       </c>
@@ -1712,7 +1710,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
@@ -1735,8 +1733,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000 •• PROTECTED 関係者外秘&amp;1#_x000D_</oddHeader>
-  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{2c7890e8-8459-473b-8b86-643375e9aab5}" enabled="1" method="Privileged" siteId="{8c642d1d-d709-47b0-ab10-080af10798fb}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>